<commit_message>
minor changes , tool working for Performance Testing on both Get and Post API's
</commit_message>
<xml_diff>
--- a/perfMonitoringApp/results/nullPerfResults-Highlighted.xlsx
+++ b/perfMonitoringApp/results/nullPerfResults-Highlighted.xlsx
@@ -12,15 +12,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="239">
-  <si>
-    <t>1568655041320</t>
-  </si>
-  <si>
-    <t>1230</t>
-  </si>
-  <si>
-    <t>taxPolicyApiTest</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="189">
+  <si>
+    <t>1568897339208</t>
+  </si>
+  <si>
+    <t>3300</t>
+  </si>
+  <si>
+    <t>taxPolicyLoadTest</t>
   </si>
   <si>
     <t>200</t>
@@ -29,706 +29,556 @@
     <t>OK</t>
   </si>
   <si>
+    <t>Thread Group 1-5</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>2407</t>
+  </si>
+  <si>
+    <t>1023</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>https://ccrs-qa-api.reztrip.io/cc/taxAndPolicyDetails</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>2478</t>
+  </si>
+  <si>
+    <t>3299</t>
+  </si>
+  <si>
+    <t>Thread Group 1-18</t>
+  </si>
+  <si>
+    <t>2369</t>
+  </si>
+  <si>
+    <t>3296</t>
+  </si>
+  <si>
+    <t>2482</t>
+  </si>
+  <si>
+    <t>1568897339215</t>
+  </si>
+  <si>
+    <t>3292</t>
+  </si>
+  <si>
+    <t>Thread Group 1-7</t>
+  </si>
+  <si>
+    <t>2469</t>
+  </si>
+  <si>
+    <t>1568897339418</t>
+  </si>
+  <si>
+    <t>3091</t>
+  </si>
+  <si>
+    <t>Thread Group 1-40</t>
+  </si>
+  <si>
+    <t>3090</t>
+  </si>
+  <si>
+    <t>2249</t>
+  </si>
+  <si>
+    <t>1568897339256</t>
+  </si>
+  <si>
+    <t>3253</t>
+  </si>
+  <si>
+    <t>Thread Group 1-32</t>
+  </si>
+  <si>
+    <t>2410</t>
+  </si>
+  <si>
+    <t>1568897339618</t>
+  </si>
+  <si>
+    <t>2891</t>
+  </si>
+  <si>
+    <t>Thread Group 1-50</t>
+  </si>
+  <si>
+    <t>2060</t>
+  </si>
+  <si>
+    <t>1568897339222</t>
+  </si>
+  <si>
+    <t>3285</t>
+  </si>
+  <si>
+    <t>Thread Group 1-29</t>
+  </si>
+  <si>
+    <t>2456</t>
+  </si>
+  <si>
+    <t>3301</t>
+  </si>
+  <si>
+    <t>Thread Group 1-20</t>
+  </si>
+  <si>
+    <t>2466</t>
+  </si>
+  <si>
+    <t>1568897339236</t>
+  </si>
+  <si>
+    <t>3270</t>
+  </si>
+  <si>
+    <t>Thread Group 1-31</t>
+  </si>
+  <si>
+    <t>2434</t>
+  </si>
+  <si>
+    <t>1568897339214</t>
+  </si>
+  <si>
+    <t>3293</t>
+  </si>
+  <si>
+    <t>Thread Group 1-4</t>
+  </si>
+  <si>
+    <t>2453</t>
+  </si>
+  <si>
+    <t>1568897339216</t>
+  </si>
+  <si>
+    <t>3291</t>
+  </si>
+  <si>
+    <t>Thread Group 1-8</t>
+  </si>
+  <si>
+    <t>2451</t>
+  </si>
+  <si>
+    <t>3297</t>
+  </si>
+  <si>
+    <t>Thread Group 1-14</t>
+  </si>
+  <si>
+    <t>1568897339210</t>
+  </si>
+  <si>
+    <t>3295</t>
+  </si>
+  <si>
+    <t>Thread Group 1-28</t>
+  </si>
+  <si>
+    <t>3294</t>
+  </si>
+  <si>
+    <t>2465</t>
+  </si>
+  <si>
+    <t>1568897339378</t>
+  </si>
+  <si>
+    <t>3132</t>
+  </si>
+  <si>
+    <t>Thread Group 1-38</t>
+  </si>
+  <si>
+    <t>2297</t>
+  </si>
+  <si>
+    <t>Thread Group 1-23</t>
+  </si>
+  <si>
+    <t>2464</t>
+  </si>
+  <si>
+    <t>3290</t>
+  </si>
+  <si>
     <t>Thread Group 1-19</t>
   </si>
   <si>
-    <t>text</t>
-  </si>
-  <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>2354</t>
-  </si>
-  <si>
-    <t>1039</t>
-  </si>
-  <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t>https://ccrs-qa-api.reztrip.io/cc/taxAndPolicyDetails?_ts=1568615544641</t>
-  </si>
-  <si>
-    <t>1229</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>925</t>
-  </si>
-  <si>
-    <t>1568655041261</t>
-  </si>
-  <si>
-    <t>1640</t>
-  </si>
-  <si>
-    <t>400</t>
-  </si>
-  <si>
-    <t>Bad Request</t>
+    <t>2468</t>
+  </si>
+  <si>
+    <t>1568897339495</t>
+  </si>
+  <si>
+    <t>3011</t>
+  </si>
+  <si>
+    <t>Thread Group 1-44</t>
+  </si>
+  <si>
+    <t>2183</t>
+  </si>
+  <si>
+    <t>1568897339276</t>
+  </si>
+  <si>
+    <t>3229</t>
+  </si>
+  <si>
+    <t>Thread Group 1-33</t>
+  </si>
+  <si>
+    <t>3228</t>
+  </si>
+  <si>
+    <t>2403</t>
+  </si>
+  <si>
+    <t>1568897339323</t>
+  </si>
+  <si>
+    <t>3183</t>
+  </si>
+  <si>
+    <t>Thread Group 1-36</t>
+  </si>
+  <si>
+    <t>2358</t>
+  </si>
+  <si>
+    <t>1568897339212</t>
+  </si>
+  <si>
+    <t>Thread Group 1-12</t>
+  </si>
+  <si>
+    <t>2470</t>
+  </si>
+  <si>
+    <t>1568897339211</t>
+  </si>
+  <si>
+    <t>Thread Group 1-24</t>
+  </si>
+  <si>
+    <t>2463</t>
+  </si>
+  <si>
+    <t>3302</t>
+  </si>
+  <si>
+    <t>Thread Group 1-13</t>
+  </si>
+  <si>
+    <t>1568897339292</t>
+  </si>
+  <si>
+    <t>3214</t>
+  </si>
+  <si>
+    <t>Thread Group 1-34</t>
+  </si>
+  <si>
+    <t>3212</t>
+  </si>
+  <si>
+    <t>2375</t>
+  </si>
+  <si>
+    <t>1568897339510</t>
+  </si>
+  <si>
+    <t>2995</t>
+  </si>
+  <si>
+    <t>Thread Group 1-45</t>
+  </si>
+  <si>
+    <t>2156</t>
+  </si>
+  <si>
+    <t>Thread Group 1-17</t>
+  </si>
+  <si>
+    <t>2480</t>
+  </si>
+  <si>
+    <t>1568897339447</t>
+  </si>
+  <si>
+    <t>3059</t>
+  </si>
+  <si>
+    <t>Thread Group 1-42</t>
+  </si>
+  <si>
+    <t>3058</t>
+  </si>
+  <si>
+    <t>2229</t>
+  </si>
+  <si>
+    <t>3298</t>
+  </si>
+  <si>
+    <t>Thread Group 1-9</t>
+  </si>
+  <si>
+    <t>2461</t>
+  </si>
+  <si>
+    <t>Thread Group 1-26</t>
+  </si>
+  <si>
+    <t>2460</t>
+  </si>
+  <si>
+    <t>1568897339224</t>
+  </si>
+  <si>
+    <t>3281</t>
+  </si>
+  <si>
+    <t>Thread Group 1-10</t>
+  </si>
+  <si>
+    <t>3280</t>
+  </si>
+  <si>
+    <t>2446</t>
+  </si>
+  <si>
+    <t>Thread Group 1-11</t>
+  </si>
+  <si>
+    <t>1568897339217</t>
+  </si>
+  <si>
+    <t>3289</t>
+  </si>
+  <si>
+    <t>Thread Group 1-6</t>
+  </si>
+  <si>
+    <t>2449</t>
+  </si>
+  <si>
+    <t>Thread Group 1-25</t>
+  </si>
+  <si>
+    <t>2457</t>
+  </si>
+  <si>
+    <t>1568897339356</t>
+  </si>
+  <si>
+    <t>3155</t>
+  </si>
+  <si>
+    <t>Thread Group 1-37</t>
+  </si>
+  <si>
+    <t>2320</t>
+  </si>
+  <si>
+    <t>1568897339572</t>
+  </si>
+  <si>
+    <t>2933</t>
+  </si>
+  <si>
+    <t>Thread Group 1-49</t>
+  </si>
+  <si>
+    <t>2932</t>
+  </si>
+  <si>
+    <t>2107</t>
+  </si>
+  <si>
+    <t>Thread Group 1-15</t>
+  </si>
+  <si>
+    <t>2473</t>
+  </si>
+  <si>
+    <t>Thread Group 1-22</t>
+  </si>
+  <si>
+    <t>Thread Group 1-2</t>
+  </si>
+  <si>
+    <t>2459</t>
+  </si>
+  <si>
+    <t>Thread Group 1-21</t>
+  </si>
+  <si>
+    <t>2471</t>
+  </si>
+  <si>
+    <t>1568897339223</t>
+  </si>
+  <si>
+    <t>3284</t>
   </si>
   <si>
     <t>Thread Group 1-16</t>
   </si>
   <si>
-    <t>false</t>
-  </si>
-  <si>
-    <t>10315</t>
-  </si>
-  <si>
-    <t>327</t>
+    <t>2445</t>
+  </si>
+  <si>
+    <t>Thread Group 1-3</t>
+  </si>
+  <si>
+    <t>1568897339553</t>
+  </si>
+  <si>
+    <t>2959</t>
+  </si>
+  <si>
+    <t>Thread Group 1-47</t>
+  </si>
+  <si>
+    <t>2113</t>
+  </si>
+  <si>
+    <t>1568897339312</t>
+  </si>
+  <si>
+    <t>3200</t>
+  </si>
+  <si>
+    <t>Thread Group 1-35</t>
+  </si>
+  <si>
+    <t>2366</t>
+  </si>
+  <si>
+    <t>1568897339213</t>
+  </si>
+  <si>
+    <t>Thread Group 1-27</t>
   </si>
   <si>
     <t>49</t>
   </si>
   <si>
-    <t>983</t>
-  </si>
-  <si>
-    <t>1568655041763</t>
-  </si>
-  <si>
-    <t>1151</t>
-  </si>
-  <si>
-    <t>Thread Group 1-42</t>
-  </si>
-  <si>
-    <t>2854</t>
-  </si>
-  <si>
-    <t>1041</t>
-  </si>
-  <si>
-    <t>48</t>
-  </si>
-  <si>
-    <t>484</t>
-  </si>
-  <si>
-    <t>1568655041537</t>
-  </si>
-  <si>
-    <t>1380</t>
+    <t>1568897339228</t>
   </si>
   <si>
     <t>Thread Group 1-30</t>
   </si>
   <si>
-    <t>2392</t>
-  </si>
-  <si>
-    <t>47</t>
-  </si>
-  <si>
-    <t>707</t>
-  </si>
-  <si>
-    <t>1568655041196</t>
-  </si>
-  <si>
-    <t>1722</t>
-  </si>
-  <si>
-    <t>Thread Group 1-7</t>
-  </si>
-  <si>
-    <t>1050</t>
-  </si>
-  <si>
-    <t>1568655041401</t>
-  </si>
-  <si>
-    <t>1517</t>
-  </si>
-  <si>
-    <t>Thread Group 1-23</t>
-  </si>
-  <si>
-    <t>845</t>
-  </si>
-  <si>
-    <t>1568655041894</t>
-  </si>
-  <si>
-    <t>1026</t>
-  </si>
-  <si>
-    <t>Thread Group 1-49</t>
-  </si>
-  <si>
-    <t>1051</t>
-  </si>
-  <si>
-    <t>44</t>
-  </si>
-  <si>
-    <t>349</t>
-  </si>
-  <si>
-    <t>1568655041839</t>
-  </si>
-  <si>
-    <t>1082</t>
+    <t>37</t>
+  </si>
+  <si>
+    <t>1568897339533</t>
+  </si>
+  <si>
+    <t>2986</t>
   </si>
   <si>
     <t>Thread Group 1-46</t>
   </si>
   <si>
-    <t>43</t>
-  </si>
-  <si>
-    <t>408</t>
-  </si>
-  <si>
-    <t>1568655041572</t>
-  </si>
-  <si>
-    <t>1356</t>
-  </si>
-  <si>
-    <t>Thread Group 1-32</t>
-  </si>
-  <si>
-    <t>42</t>
-  </si>
-  <si>
-    <t>1355</t>
-  </si>
-  <si>
-    <t>679</t>
-  </si>
-  <si>
-    <t>1568655041195</t>
-  </si>
-  <si>
-    <t>1745</t>
-  </si>
-  <si>
-    <t>Thread Group 1-8</t>
-  </si>
-  <si>
-    <t>41</t>
-  </si>
-  <si>
-    <t>1055</t>
-  </si>
-  <si>
-    <t>1568655041781</t>
-  </si>
-  <si>
-    <t>1167</t>
+    <t>2142</t>
+  </si>
+  <si>
+    <t>1568897339402</t>
+  </si>
+  <si>
+    <t>3121</t>
+  </si>
+  <si>
+    <t>Thread Group 1-39</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>2277</t>
+  </si>
+  <si>
+    <t>1568897339474</t>
+  </si>
+  <si>
+    <t>3050</t>
   </si>
   <si>
     <t>Thread Group 1-43</t>
   </si>
   <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>464</t>
-  </si>
-  <si>
-    <t>1568655041208</t>
-  </si>
-  <si>
-    <t>1747</t>
-  </si>
-  <si>
-    <t>Thread Group 1-13</t>
-  </si>
-  <si>
-    <t>39</t>
-  </si>
-  <si>
-    <t>1763</t>
-  </si>
-  <si>
-    <t>Thread Group 1-2</t>
-  </si>
-  <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>1054</t>
-  </si>
-  <si>
-    <t>1568655041421</t>
-  </si>
-  <si>
-    <t>1539</t>
-  </si>
-  <si>
-    <t>Thread Group 1-24</t>
-  </si>
-  <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>831</t>
-  </si>
-  <si>
-    <t>1767</t>
-  </si>
-  <si>
-    <t>Thread Group 1-5</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>1568655041746</t>
-  </si>
-  <si>
-    <t>1216</t>
+    <t>20</t>
+  </si>
+  <si>
+    <t>3046</t>
+  </si>
+  <si>
+    <t>2199</t>
+  </si>
+  <si>
+    <t>1568897339416</t>
+  </si>
+  <si>
+    <t>3127</t>
   </si>
   <si>
     <t>Thread Group 1-41</t>
   </si>
   <si>
-    <t>498</t>
-  </si>
-  <si>
-    <t>1769</t>
-  </si>
-  <si>
-    <t>Thread Group 1-10</t>
-  </si>
-  <si>
-    <t>2816</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>1768</t>
-  </si>
-  <si>
-    <t>1053</t>
-  </si>
-  <si>
-    <t>1568655041230</t>
-  </si>
-  <si>
-    <t>1734</t>
-  </si>
-  <si>
-    <t>Thread Group 1-14</t>
-  </si>
-  <si>
-    <t>1021</t>
-  </si>
-  <si>
-    <t>1568655041557</t>
-  </si>
-  <si>
-    <t>1408</t>
-  </si>
-  <si>
-    <t>Thread Group 1-31</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>689</t>
-  </si>
-  <si>
-    <t>1770</t>
-  </si>
-  <si>
-    <t>Thread Group 1-11</t>
-  </si>
-  <si>
-    <t>1568655041242</t>
-  </si>
-  <si>
-    <t>1724</t>
-  </si>
-  <si>
-    <t>Thread Group 1-15</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>1007</t>
-  </si>
-  <si>
-    <t>1568655041462</t>
-  </si>
-  <si>
-    <t>1505</t>
-  </si>
-  <si>
-    <t>Thread Group 1-26</t>
-  </si>
-  <si>
-    <t>789</t>
-  </si>
-  <si>
-    <t>1568655041725</t>
-  </si>
-  <si>
-    <t>1243</t>
-  </si>
-  <si>
-    <t>Thread Group 1-40</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>527</t>
-  </si>
-  <si>
-    <t>1773</t>
-  </si>
-  <si>
-    <t>Thread Group 1-3</t>
-  </si>
-  <si>
-    <t>1568655041359</t>
-  </si>
-  <si>
-    <t>1609</t>
-  </si>
-  <si>
-    <t>Thread Group 1-21</t>
-  </si>
-  <si>
-    <t>898</t>
-  </si>
-  <si>
-    <t>1568655041520</t>
-  </si>
-  <si>
-    <t>1451</t>
-  </si>
-  <si>
-    <t>Thread Group 1-29</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>730</t>
-  </si>
-  <si>
-    <t>1568655041501</t>
-  </si>
-  <si>
-    <t>1477</t>
-  </si>
-  <si>
-    <t>Thread Group 1-28</t>
-  </si>
-  <si>
-    <t>1043</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>750</t>
-  </si>
-  <si>
-    <t>1783</t>
-  </si>
-  <si>
-    <t>Thread Group 1-9</t>
-  </si>
-  <si>
-    <t>1048</t>
-  </si>
-  <si>
-    <t>1786</t>
-  </si>
-  <si>
-    <t>Thread Group 1-6</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>1788</t>
-  </si>
-  <si>
-    <t>Thread Group 1-4</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>1568655041303</t>
-  </si>
-  <si>
-    <t>1681</t>
-  </si>
-  <si>
-    <t>Thread Group 1-18</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>944</t>
-  </si>
-  <si>
-    <t>1568655041855</t>
-  </si>
-  <si>
-    <t>1130</t>
-  </si>
-  <si>
-    <t>Thread Group 1-47</t>
-  </si>
-  <si>
-    <t>396</t>
-  </si>
-  <si>
-    <t>1568655041878</t>
-  </si>
-  <si>
-    <t>1126</t>
+    <t>3</t>
+  </si>
+  <si>
+    <t>2255</t>
+  </si>
+  <si>
+    <t>1568897339550</t>
+  </si>
+  <si>
+    <t>2999</t>
   </si>
   <si>
     <t>Thread Group 1-48</t>
   </si>
   <si>
-    <t>10316</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>372</t>
-  </si>
-  <si>
-    <t>1568655041652</t>
-  </si>
-  <si>
-    <t>1357</t>
-  </si>
-  <si>
-    <t>Thread Group 1-36</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>601</t>
-  </si>
-  <si>
-    <t>1814</t>
+    <t>2</t>
+  </si>
+  <si>
+    <t>2137</t>
+  </si>
+  <si>
+    <t>3461</t>
   </si>
   <si>
     <t>Thread Group 1-1</t>
   </si>
   <si>
-    <t>1821</t>
-  </si>
-  <si>
-    <t>Thread Group 1-12</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>1049</t>
-  </si>
-  <si>
-    <t>1568655041802</t>
-  </si>
-  <si>
-    <t>1218</t>
-  </si>
-  <si>
-    <t>Thread Group 1-44</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>450</t>
-  </si>
-  <si>
-    <t>1568655041819</t>
-  </si>
-  <si>
-    <t>1201</t>
-  </si>
-  <si>
-    <t>Thread Group 1-45</t>
-  </si>
-  <si>
-    <t>435</t>
-  </si>
-  <si>
-    <t>1568655041703</t>
-  </si>
-  <si>
-    <t>1321</t>
-  </si>
-  <si>
-    <t>Thread Group 1-39</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>541</t>
-  </si>
-  <si>
-    <t>1568655041481</t>
-  </si>
-  <si>
-    <t>1544</t>
-  </si>
-  <si>
-    <t>Thread Group 1-27</t>
-  </si>
-  <si>
-    <t>1543</t>
-  </si>
-  <si>
-    <t>766</t>
-  </si>
-  <si>
-    <t>1568655041337</t>
-  </si>
-  <si>
-    <t>1688</t>
-  </si>
-  <si>
-    <t>Thread Group 1-20</t>
-  </si>
-  <si>
-    <t>915</t>
-  </si>
-  <si>
-    <t>1568655041602</t>
-  </si>
-  <si>
-    <t>1422</t>
-  </si>
-  <si>
-    <t>Thread Group 1-33</t>
-  </si>
-  <si>
-    <t>640</t>
-  </si>
-  <si>
-    <t>1568655041614</t>
-  </si>
-  <si>
-    <t>1413</t>
-  </si>
-  <si>
-    <t>Thread Group 1-34</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>631</t>
-  </si>
-  <si>
-    <t>1568655041683</t>
-  </si>
-  <si>
-    <t>1344</t>
-  </si>
-  <si>
-    <t>Thread Group 1-38</t>
-  </si>
-  <si>
-    <t>567</t>
-  </si>
-  <si>
-    <t>1568655041634</t>
-  </si>
-  <si>
-    <t>1394</t>
-  </si>
-  <si>
-    <t>Thread Group 1-35</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>614</t>
-  </si>
-  <si>
-    <t>1568655041441</t>
-  </si>
-  <si>
-    <t>1588</t>
-  </si>
-  <si>
-    <t>Thread Group 1-25</t>
-  </si>
-  <si>
-    <t>806</t>
-  </si>
-  <si>
-    <t>1568655041673</t>
-  </si>
-  <si>
-    <t>Thread Group 1-37</t>
-  </si>
-  <si>
-    <t>575</t>
-  </si>
-  <si>
-    <t>1568655041377</t>
-  </si>
-  <si>
-    <t>1653</t>
-  </si>
-  <si>
-    <t>Thread Group 1-22</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>871</t>
-  </si>
-  <si>
-    <t>1568655041281</t>
-  </si>
-  <si>
-    <t>1749</t>
-  </si>
-  <si>
-    <t>Thread Group 1-17</t>
-  </si>
-  <si>
-    <t>974</t>
-  </si>
-  <si>
-    <t>1568655041916</t>
-  </si>
-  <si>
-    <t>1115</t>
-  </si>
-  <si>
-    <t>Thread Group 1-50</t>
-  </si>
-  <si>
     <t>1</t>
-  </si>
-  <si>
-    <t>334</t>
   </si>
 </sst>
 </file>
@@ -845,74 +695,74 @@
         <v>12</v>
       </c>
       <c r="O1" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="P1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" t="s">
         <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" t="s">
+      <c r="P2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q2" t="s">
         <v>19</v>
-      </c>
-      <c r="F2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2" t="s">
-        <v>24</v>
-      </c>
-      <c r="N2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O2" t="s">
-        <v>17</v>
-      </c>
-      <c r="P2" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -924,7 +774,7 @@
         <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="G3" t="s">
         <v>6</v>
@@ -936,36 +786,36 @@
         <v>8</v>
       </c>
       <c r="J3" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="K3" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="L3" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="M3" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="N3" t="s">
         <v>12</v>
       </c>
       <c r="O3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="P3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -977,7 +827,7 @@
         <v>4</v>
       </c>
       <c r="F4" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="G4" t="s">
         <v>6</v>
@@ -989,36 +839,36 @@
         <v>8</v>
       </c>
       <c r="J4" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="K4" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="L4" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="M4" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="N4" t="s">
         <v>12</v>
       </c>
       <c r="O4" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="P4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q4" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -1030,7 +880,7 @@
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="G5" t="s">
         <v>6</v>
@@ -1042,36 +892,36 @@
         <v>8</v>
       </c>
       <c r="J5" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="K5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O5" t="s">
         <v>30</v>
       </c>
-      <c r="L5" t="s">
-        <v>37</v>
-      </c>
-      <c r="M5" t="s">
-        <v>37</v>
-      </c>
-      <c r="N5" t="s">
-        <v>12</v>
-      </c>
-      <c r="O5" t="s">
-        <v>40</v>
-      </c>
       <c r="P5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q5" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
@@ -1083,7 +933,7 @@
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="G6" t="s">
         <v>6</v>
@@ -1095,36 +945,36 @@
         <v>8</v>
       </c>
       <c r="J6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L6" t="s">
+        <v>11</v>
+      </c>
+      <c r="M6" t="s">
+        <v>11</v>
+      </c>
+      <c r="N6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O6" t="s">
+        <v>34</v>
+      </c>
+      <c r="P6" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q6" t="s">
         <v>36</v>
-      </c>
-      <c r="K6" t="s">
-        <v>30</v>
-      </c>
-      <c r="L6" t="s">
-        <v>37</v>
-      </c>
-      <c r="M6" t="s">
-        <v>37</v>
-      </c>
-      <c r="N6" t="s">
-        <v>12</v>
-      </c>
-      <c r="O6" t="s">
-        <v>44</v>
-      </c>
-      <c r="P6" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -1136,7 +986,7 @@
         <v>4</v>
       </c>
       <c r="F7" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="G7" t="s">
         <v>6</v>
@@ -1148,36 +998,36 @@
         <v>8</v>
       </c>
       <c r="J7" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="K7" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="L7" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="M7" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="N7" t="s">
         <v>12</v>
       </c>
       <c r="O7" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="P7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q7" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -1189,7 +1039,7 @@
         <v>4</v>
       </c>
       <c r="F8" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="G8" t="s">
         <v>6</v>
@@ -1204,86 +1054,86 @@
         <v>9</v>
       </c>
       <c r="K8" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="L8" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="M8" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="N8" t="s">
         <v>12</v>
       </c>
       <c r="O8" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="P8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q8" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="F9" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="G9" t="s">
         <v>6</v>
       </c>
       <c r="H9" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="I9" t="s">
         <v>8</v>
       </c>
       <c r="J9" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="K9" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="L9" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="M9" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="N9" t="s">
         <v>12</v>
       </c>
       <c r="O9" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="P9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q9" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="C10" t="s">
         <v>2</v>
@@ -1295,7 +1145,7 @@
         <v>4</v>
       </c>
       <c r="F10" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="G10" t="s">
         <v>6</v>
@@ -1307,36 +1157,36 @@
         <v>8</v>
       </c>
       <c r="J10" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="K10" t="s">
         <v>10</v>
       </c>
       <c r="L10" t="s">
-        <v>67</v>
+        <v>11</v>
       </c>
       <c r="M10" t="s">
-        <v>67</v>
+        <v>11</v>
       </c>
       <c r="N10" t="s">
         <v>12</v>
       </c>
       <c r="O10" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="P10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q10" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="B11" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -1348,7 +1198,7 @@
         <v>4</v>
       </c>
       <c r="F11" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="G11" t="s">
         <v>6</v>
@@ -1363,33 +1213,33 @@
         <v>9</v>
       </c>
       <c r="K11" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="L11" t="s">
-        <v>72</v>
+        <v>11</v>
       </c>
       <c r="M11" t="s">
-        <v>72</v>
+        <v>11</v>
       </c>
       <c r="N11" t="s">
         <v>12</v>
       </c>
       <c r="O11" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="P11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q11" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
@@ -1401,7 +1251,7 @@
         <v>4</v>
       </c>
       <c r="F12" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="G12" t="s">
         <v>6</v>
@@ -1413,36 +1263,36 @@
         <v>8</v>
       </c>
       <c r="J12" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="K12" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="L12" t="s">
-        <v>77</v>
+        <v>11</v>
       </c>
       <c r="M12" t="s">
-        <v>77</v>
+        <v>11</v>
       </c>
       <c r="N12" t="s">
         <v>12</v>
       </c>
       <c r="O12" t="s">
-        <v>75</v>
+        <v>18</v>
       </c>
       <c r="P12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q12" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="B13" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
@@ -1454,7 +1304,7 @@
         <v>4</v>
       </c>
       <c r="F13" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="G13" t="s">
         <v>6</v>
@@ -1466,36 +1316,36 @@
         <v>8</v>
       </c>
       <c r="J13" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="K13" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="L13" t="s">
-        <v>80</v>
+        <v>11</v>
       </c>
       <c r="M13" t="s">
-        <v>80</v>
+        <v>11</v>
       </c>
       <c r="N13" t="s">
         <v>12</v>
       </c>
       <c r="O13" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="P13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q13" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="B14" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
@@ -1507,7 +1357,7 @@
         <v>4</v>
       </c>
       <c r="F14" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="G14" t="s">
         <v>6</v>
@@ -1525,30 +1375,30 @@
         <v>10</v>
       </c>
       <c r="L14" t="s">
-        <v>85</v>
+        <v>11</v>
       </c>
       <c r="M14" t="s">
-        <v>85</v>
+        <v>11</v>
       </c>
       <c r="N14" t="s">
         <v>12</v>
       </c>
       <c r="O14" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="P14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q14" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>87</v>
+        <v>59</v>
       </c>
       <c r="C15" t="s">
         <v>2</v>
@@ -1560,7 +1410,7 @@
         <v>4</v>
       </c>
       <c r="F15" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="G15" t="s">
         <v>6</v>
@@ -1572,36 +1422,36 @@
         <v>8</v>
       </c>
       <c r="J15" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="K15" t="s">
         <v>10</v>
       </c>
       <c r="L15" t="s">
-        <v>89</v>
+        <v>11</v>
       </c>
       <c r="M15" t="s">
-        <v>89</v>
+        <v>11</v>
       </c>
       <c r="N15" t="s">
         <v>12</v>
       </c>
       <c r="O15" t="s">
-        <v>87</v>
+        <v>59</v>
       </c>
       <c r="P15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q15" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>90</v>
+        <v>52</v>
       </c>
       <c r="B16" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
@@ -1613,7 +1463,7 @@
         <v>4</v>
       </c>
       <c r="F16" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="G16" t="s">
         <v>6</v>
@@ -1625,36 +1475,36 @@
         <v>8</v>
       </c>
       <c r="J16" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="K16" t="s">
         <v>10</v>
       </c>
       <c r="L16" t="s">
-        <v>89</v>
+        <v>11</v>
       </c>
       <c r="M16" t="s">
-        <v>89</v>
+        <v>11</v>
       </c>
       <c r="N16" t="s">
         <v>12</v>
       </c>
       <c r="O16" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="P16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q16" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B17" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
@@ -1666,7 +1516,7 @@
         <v>4</v>
       </c>
       <c r="F17" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="G17" t="s">
         <v>6</v>
@@ -1678,36 +1528,36 @@
         <v>8</v>
       </c>
       <c r="J17" t="s">
-        <v>96</v>
+        <v>17</v>
       </c>
       <c r="K17" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="L17" t="s">
-        <v>97</v>
+        <v>11</v>
       </c>
       <c r="M17" t="s">
-        <v>97</v>
+        <v>11</v>
       </c>
       <c r="N17" t="s">
         <v>12</v>
       </c>
       <c r="O17" t="s">
-        <v>98</v>
+        <v>73</v>
       </c>
       <c r="P17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q17" t="s">
-        <v>99</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="B18" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
       <c r="C18" t="s">
         <v>2</v>
@@ -1719,7 +1569,7 @@
         <v>4</v>
       </c>
       <c r="F18" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="G18" t="s">
         <v>6</v>
@@ -1731,36 +1581,36 @@
         <v>8</v>
       </c>
       <c r="J18" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="K18" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="L18" t="s">
-        <v>97</v>
+        <v>11</v>
       </c>
       <c r="M18" t="s">
-        <v>97</v>
+        <v>11</v>
       </c>
       <c r="N18" t="s">
         <v>12</v>
       </c>
       <c r="O18" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="P18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q18" t="s">
-        <v>103</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="B19" t="s">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="C19" t="s">
         <v>2</v>
@@ -1772,7 +1622,7 @@
         <v>4</v>
       </c>
       <c r="F19" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="G19" t="s">
         <v>6</v>
@@ -1784,36 +1634,36 @@
         <v>8</v>
       </c>
       <c r="J19" t="s">
-        <v>96</v>
+        <v>17</v>
       </c>
       <c r="K19" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="L19" t="s">
-        <v>107</v>
+        <v>11</v>
       </c>
       <c r="M19" t="s">
-        <v>107</v>
+        <v>11</v>
       </c>
       <c r="N19" t="s">
         <v>12</v>
       </c>
       <c r="O19" t="s">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="P19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q19" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="B20" t="s">
-        <v>109</v>
+        <v>49</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
@@ -1825,7 +1675,7 @@
         <v>4</v>
       </c>
       <c r="F20" t="s">
-        <v>110</v>
+        <v>86</v>
       </c>
       <c r="G20" t="s">
         <v>6</v>
@@ -1837,36 +1687,36 @@
         <v>8</v>
       </c>
       <c r="J20" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="K20" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="L20" t="s">
-        <v>107</v>
+        <v>11</v>
       </c>
       <c r="M20" t="s">
-        <v>107</v>
+        <v>11</v>
       </c>
       <c r="N20" t="s">
         <v>12</v>
       </c>
       <c r="O20" t="s">
-        <v>109</v>
+        <v>49</v>
       </c>
       <c r="P20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q20" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="B21" t="s">
-        <v>112</v>
+        <v>61</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
@@ -1878,7 +1728,7 @@
         <v>4</v>
       </c>
       <c r="F21" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
       <c r="G21" t="s">
         <v>6</v>
@@ -1890,36 +1740,36 @@
         <v>8</v>
       </c>
       <c r="J21" t="s">
-        <v>96</v>
+        <v>17</v>
       </c>
       <c r="K21" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="L21" t="s">
-        <v>114</v>
+        <v>11</v>
       </c>
       <c r="M21" t="s">
-        <v>114</v>
+        <v>11</v>
       </c>
       <c r="N21" t="s">
         <v>12</v>
       </c>
       <c r="O21" t="s">
-        <v>112</v>
+        <v>61</v>
       </c>
       <c r="P21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q21" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>116</v>
+        <v>0</v>
       </c>
       <c r="B22" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="C22" t="s">
         <v>2</v>
@@ -1931,7 +1781,7 @@
         <v>4</v>
       </c>
       <c r="F22" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="G22" t="s">
         <v>6</v>
@@ -1943,36 +1793,36 @@
         <v>8</v>
       </c>
       <c r="J22" t="s">
-        <v>96</v>
+        <v>17</v>
       </c>
       <c r="K22" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="L22" t="s">
-        <v>114</v>
+        <v>11</v>
       </c>
       <c r="M22" t="s">
-        <v>114</v>
+        <v>11</v>
       </c>
       <c r="N22" t="s">
         <v>12</v>
       </c>
       <c r="O22" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="P22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q22" t="s">
-        <v>119</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>120</v>
+        <v>93</v>
       </c>
       <c r="B23" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="C23" t="s">
         <v>2</v>
@@ -1984,7 +1834,7 @@
         <v>4</v>
       </c>
       <c r="F23" t="s">
-        <v>122</v>
+        <v>95</v>
       </c>
       <c r="G23" t="s">
         <v>6</v>
@@ -2002,30 +1852,30 @@
         <v>10</v>
       </c>
       <c r="L23" t="s">
-        <v>123</v>
+        <v>11</v>
       </c>
       <c r="M23" t="s">
-        <v>123</v>
+        <v>11</v>
       </c>
       <c r="N23" t="s">
         <v>12</v>
       </c>
       <c r="O23" t="s">
-        <v>121</v>
+        <v>96</v>
       </c>
       <c r="P23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q23" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>98</v>
       </c>
       <c r="B24" t="s">
-        <v>125</v>
+        <v>99</v>
       </c>
       <c r="C24" t="s">
         <v>2</v>
@@ -2037,7 +1887,7 @@
         <v>4</v>
       </c>
       <c r="F24" t="s">
-        <v>126</v>
+        <v>100</v>
       </c>
       <c r="G24" t="s">
         <v>6</v>
@@ -2055,30 +1905,30 @@
         <v>10</v>
       </c>
       <c r="L24" t="s">
-        <v>123</v>
+        <v>11</v>
       </c>
       <c r="M24" t="s">
-        <v>123</v>
+        <v>11</v>
       </c>
       <c r="N24" t="s">
         <v>12</v>
       </c>
       <c r="O24" t="s">
-        <v>125</v>
+        <v>99</v>
       </c>
       <c r="P24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q24" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>127</v>
+        <v>58</v>
       </c>
       <c r="B25" t="s">
-        <v>128</v>
+        <v>18</v>
       </c>
       <c r="C25" t="s">
         <v>2</v>
@@ -2090,7 +1940,7 @@
         <v>4</v>
       </c>
       <c r="F25" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="G25" t="s">
         <v>6</v>
@@ -2108,30 +1958,30 @@
         <v>10</v>
       </c>
       <c r="L25" t="s">
-        <v>123</v>
+        <v>11</v>
       </c>
       <c r="M25" t="s">
-        <v>123</v>
+        <v>11</v>
       </c>
       <c r="N25" t="s">
         <v>12</v>
       </c>
       <c r="O25" t="s">
-        <v>128</v>
+        <v>59</v>
       </c>
       <c r="P25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q25" t="s">
-        <v>130</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>131</v>
+        <v>104</v>
       </c>
       <c r="B26" t="s">
-        <v>132</v>
+        <v>105</v>
       </c>
       <c r="C26" t="s">
         <v>2</v>
@@ -2143,7 +1993,7 @@
         <v>4</v>
       </c>
       <c r="F26" t="s">
-        <v>133</v>
+        <v>106</v>
       </c>
       <c r="G26" t="s">
         <v>6</v>
@@ -2155,36 +2005,36 @@
         <v>8</v>
       </c>
       <c r="J26" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="K26" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="L26" t="s">
-        <v>134</v>
+        <v>11</v>
       </c>
       <c r="M26" t="s">
-        <v>134</v>
+        <v>11</v>
       </c>
       <c r="N26" t="s">
         <v>12</v>
       </c>
       <c r="O26" t="s">
-        <v>132</v>
+        <v>107</v>
       </c>
       <c r="P26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q26" t="s">
-        <v>135</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>136</v>
+        <v>0</v>
       </c>
       <c r="B27" t="s">
-        <v>137</v>
+        <v>109</v>
       </c>
       <c r="C27" t="s">
         <v>2</v>
@@ -2196,7 +2046,7 @@
         <v>4</v>
       </c>
       <c r="F27" t="s">
-        <v>138</v>
+        <v>110</v>
       </c>
       <c r="G27" t="s">
         <v>6</v>
@@ -2211,33 +2061,33 @@
         <v>9</v>
       </c>
       <c r="K27" t="s">
-        <v>139</v>
+        <v>10</v>
       </c>
       <c r="L27" t="s">
-        <v>140</v>
+        <v>11</v>
       </c>
       <c r="M27" t="s">
-        <v>140</v>
+        <v>11</v>
       </c>
       <c r="N27" t="s">
         <v>12</v>
       </c>
       <c r="O27" t="s">
-        <v>137</v>
+        <v>109</v>
       </c>
       <c r="P27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q27" t="s">
-        <v>141</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="B28" t="s">
-        <v>142</v>
+        <v>15</v>
       </c>
       <c r="C28" t="s">
         <v>2</v>
@@ -2249,7 +2099,7 @@
         <v>4</v>
       </c>
       <c r="F28" t="s">
-        <v>143</v>
+        <v>112</v>
       </c>
       <c r="G28" t="s">
         <v>6</v>
@@ -2261,36 +2111,36 @@
         <v>8</v>
       </c>
       <c r="J28" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="K28" t="s">
         <v>10</v>
       </c>
       <c r="L28" t="s">
-        <v>140</v>
+        <v>11</v>
       </c>
       <c r="M28" t="s">
-        <v>140</v>
+        <v>11</v>
       </c>
       <c r="N28" t="s">
         <v>12</v>
       </c>
       <c r="O28" t="s">
-        <v>142</v>
+        <v>15</v>
       </c>
       <c r="P28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q28" t="s">
-        <v>144</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>39</v>
+        <v>114</v>
       </c>
       <c r="B29" t="s">
-        <v>145</v>
+        <v>115</v>
       </c>
       <c r="C29" t="s">
         <v>2</v>
@@ -2302,7 +2152,7 @@
         <v>4</v>
       </c>
       <c r="F29" t="s">
-        <v>146</v>
+        <v>116</v>
       </c>
       <c r="G29" t="s">
         <v>6</v>
@@ -2314,36 +2164,36 @@
         <v>8</v>
       </c>
       <c r="J29" t="s">
-        <v>96</v>
+        <v>17</v>
       </c>
       <c r="K29" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="L29" t="s">
-        <v>147</v>
+        <v>11</v>
       </c>
       <c r="M29" t="s">
-        <v>147</v>
+        <v>11</v>
       </c>
       <c r="N29" t="s">
         <v>12</v>
       </c>
       <c r="O29" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="P29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q29" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B30" t="s">
-        <v>148</v>
+        <v>53</v>
       </c>
       <c r="C30" t="s">
         <v>2</v>
@@ -2355,7 +2205,7 @@
         <v>4</v>
       </c>
       <c r="F30" t="s">
-        <v>149</v>
+        <v>119</v>
       </c>
       <c r="G30" t="s">
         <v>6</v>
@@ -2367,36 +2217,36 @@
         <v>8</v>
       </c>
       <c r="J30" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="K30" t="s">
         <v>10</v>
       </c>
       <c r="L30" t="s">
-        <v>150</v>
+        <v>11</v>
       </c>
       <c r="M30" t="s">
-        <v>150</v>
+        <v>11</v>
       </c>
       <c r="N30" t="s">
         <v>12</v>
       </c>
       <c r="O30" t="s">
-        <v>148</v>
+        <v>53</v>
       </c>
       <c r="P30" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q30" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>151</v>
+        <v>120</v>
       </c>
       <c r="B31" t="s">
-        <v>152</v>
+        <v>121</v>
       </c>
       <c r="C31" t="s">
         <v>2</v>
@@ -2408,7 +2258,7 @@
         <v>4</v>
       </c>
       <c r="F31" t="s">
-        <v>153</v>
+        <v>122</v>
       </c>
       <c r="G31" t="s">
         <v>6</v>
@@ -2420,36 +2270,36 @@
         <v>8</v>
       </c>
       <c r="J31" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="K31" t="s">
         <v>10</v>
       </c>
       <c r="L31" t="s">
-        <v>154</v>
+        <v>11</v>
       </c>
       <c r="M31" t="s">
-        <v>154</v>
+        <v>11</v>
       </c>
       <c r="N31" t="s">
         <v>12</v>
       </c>
       <c r="O31" t="s">
-        <v>152</v>
+        <v>121</v>
       </c>
       <c r="P31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q31" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>156</v>
+        <v>58</v>
       </c>
       <c r="B32" t="s">
-        <v>157</v>
+        <v>56</v>
       </c>
       <c r="C32" t="s">
         <v>2</v>
@@ -2461,7 +2311,7 @@
         <v>4</v>
       </c>
       <c r="F32" t="s">
-        <v>158</v>
+        <v>124</v>
       </c>
       <c r="G32" t="s">
         <v>6</v>
@@ -2473,89 +2323,89 @@
         <v>8</v>
       </c>
       <c r="J32" t="s">
-        <v>96</v>
+        <v>17</v>
       </c>
       <c r="K32" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="L32" t="s">
-        <v>154</v>
+        <v>11</v>
       </c>
       <c r="M32" t="s">
-        <v>154</v>
+        <v>11</v>
       </c>
       <c r="N32" t="s">
         <v>12</v>
       </c>
       <c r="O32" t="s">
-        <v>157</v>
+        <v>56</v>
       </c>
       <c r="P32" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q32" t="s">
-        <v>159</v>
+        <v>125</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>160</v>
+        <v>126</v>
       </c>
       <c r="B33" t="s">
-        <v>161</v>
+        <v>127</v>
       </c>
       <c r="C33" t="s">
         <v>2</v>
       </c>
       <c r="D33" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="E33" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="F33" t="s">
-        <v>162</v>
+        <v>128</v>
       </c>
       <c r="G33" t="s">
         <v>6</v>
       </c>
       <c r="H33" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="I33" t="s">
         <v>8</v>
       </c>
       <c r="J33" t="s">
-        <v>163</v>
+        <v>17</v>
       </c>
       <c r="K33" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="L33" t="s">
-        <v>164</v>
+        <v>11</v>
       </c>
       <c r="M33" t="s">
-        <v>164</v>
+        <v>11</v>
       </c>
       <c r="N33" t="s">
         <v>12</v>
       </c>
       <c r="O33" t="s">
-        <v>161</v>
+        <v>127</v>
       </c>
       <c r="P33" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q33" t="s">
-        <v>165</v>
+        <v>129</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>166</v>
+        <v>130</v>
       </c>
       <c r="B34" t="s">
-        <v>167</v>
+        <v>131</v>
       </c>
       <c r="C34" t="s">
         <v>2</v>
@@ -2567,7 +2417,7 @@
         <v>4</v>
       </c>
       <c r="F34" t="s">
-        <v>168</v>
+        <v>132</v>
       </c>
       <c r="G34" t="s">
         <v>6</v>
@@ -2585,30 +2435,30 @@
         <v>10</v>
       </c>
       <c r="L34" t="s">
-        <v>169</v>
+        <v>11</v>
       </c>
       <c r="M34" t="s">
-        <v>169</v>
+        <v>11</v>
       </c>
       <c r="N34" t="s">
         <v>12</v>
       </c>
       <c r="O34" t="s">
-        <v>167</v>
+        <v>133</v>
       </c>
       <c r="P34" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q34" t="s">
-        <v>170</v>
+        <v>134</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="B35" t="s">
-        <v>171</v>
+        <v>56</v>
       </c>
       <c r="C35" t="s">
         <v>2</v>
@@ -2620,7 +2470,7 @@
         <v>4</v>
       </c>
       <c r="F35" t="s">
-        <v>172</v>
+        <v>135</v>
       </c>
       <c r="G35" t="s">
         <v>6</v>
@@ -2638,83 +2488,83 @@
         <v>10</v>
       </c>
       <c r="L35" t="s">
-        <v>169</v>
+        <v>11</v>
       </c>
       <c r="M35" t="s">
-        <v>169</v>
+        <v>11</v>
       </c>
       <c r="N35" t="s">
         <v>12</v>
       </c>
       <c r="O35" t="s">
-        <v>171</v>
+        <v>56</v>
       </c>
       <c r="P35" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q35" t="s">
-        <v>68</v>
+        <v>136</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="s" s="2">
-        <v>64</v>
-      </c>
-      <c r="B36" t="s" s="2">
-        <v>173</v>
-      </c>
-      <c r="C36" t="s" s="2">
-        <v>2</v>
-      </c>
-      <c r="D36" t="s" s="2">
-        <v>3</v>
-      </c>
-      <c r="E36" t="s" s="2">
-        <v>4</v>
-      </c>
-      <c r="F36" t="s" s="2">
-        <v>174</v>
-      </c>
-      <c r="G36" t="s" s="2">
-        <v>6</v>
-      </c>
-      <c r="H36" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="I36" t="s" s="2">
-        <v>8</v>
-      </c>
-      <c r="J36" t="s" s="2">
+      <c r="A36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" t="s">
+        <v>109</v>
+      </c>
+      <c r="C36" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" t="s">
+        <v>3</v>
+      </c>
+      <c r="E36" t="s">
+        <v>4</v>
+      </c>
+      <c r="F36" t="s">
+        <v>137</v>
+      </c>
+      <c r="G36" t="s">
+        <v>6</v>
+      </c>
+      <c r="H36" t="s">
+        <v>7</v>
+      </c>
+      <c r="I36" t="s">
+        <v>8</v>
+      </c>
+      <c r="J36" t="s">
         <v>9</v>
       </c>
-      <c r="K36" t="s" s="2">
-        <v>139</v>
-      </c>
-      <c r="L36" t="s" s="2">
-        <v>175</v>
-      </c>
-      <c r="M36" t="s" s="2">
-        <v>175</v>
-      </c>
-      <c r="N36" t="s" s="2">
-        <v>12</v>
-      </c>
-      <c r="O36" t="s" s="2">
-        <v>173</v>
-      </c>
-      <c r="P36" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="Q36" t="s" s="2">
-        <v>176</v>
+      <c r="K36" t="s">
+        <v>10</v>
+      </c>
+      <c r="L36" t="s">
+        <v>11</v>
+      </c>
+      <c r="M36" t="s">
+        <v>11</v>
+      </c>
+      <c r="N36" t="s">
+        <v>12</v>
+      </c>
+      <c r="O36" t="s">
+        <v>109</v>
+      </c>
+      <c r="P36" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>177</v>
+        <v>0</v>
       </c>
       <c r="B37" t="s">
-        <v>178</v>
+        <v>1</v>
       </c>
       <c r="C37" t="s">
         <v>2</v>
@@ -2726,7 +2576,7 @@
         <v>4</v>
       </c>
       <c r="F37" t="s">
-        <v>179</v>
+        <v>138</v>
       </c>
       <c r="G37" t="s">
         <v>6</v>
@@ -2738,36 +2588,36 @@
         <v>8</v>
       </c>
       <c r="J37" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="K37" t="s">
+        <v>10</v>
+      </c>
+      <c r="L37" t="s">
+        <v>11</v>
+      </c>
+      <c r="M37" t="s">
+        <v>11</v>
+      </c>
+      <c r="N37" t="s">
+        <v>12</v>
+      </c>
+      <c r="O37" t="s">
+        <v>1</v>
+      </c>
+      <c r="P37" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q37" t="s">
         <v>139</v>
-      </c>
-      <c r="L37" t="s">
-        <v>180</v>
-      </c>
-      <c r="M37" t="s">
-        <v>180</v>
-      </c>
-      <c r="N37" t="s">
-        <v>12</v>
-      </c>
-      <c r="O37" t="s">
-        <v>178</v>
-      </c>
-      <c r="P37" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q37" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>182</v>
+        <v>88</v>
       </c>
       <c r="B38" t="s">
-        <v>183</v>
+        <v>1</v>
       </c>
       <c r="C38" t="s">
         <v>2</v>
@@ -2779,7 +2629,7 @@
         <v>4</v>
       </c>
       <c r="F38" t="s">
-        <v>184</v>
+        <v>140</v>
       </c>
       <c r="G38" t="s">
         <v>6</v>
@@ -2791,36 +2641,36 @@
         <v>8</v>
       </c>
       <c r="J38" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="K38" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="L38" t="s">
-        <v>180</v>
+        <v>11</v>
       </c>
       <c r="M38" t="s">
-        <v>180</v>
+        <v>11</v>
       </c>
       <c r="N38" t="s">
         <v>12</v>
       </c>
       <c r="O38" t="s">
-        <v>183</v>
+        <v>1</v>
       </c>
       <c r="P38" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q38" t="s">
-        <v>185</v>
+        <v>141</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>186</v>
+        <v>142</v>
       </c>
       <c r="B39" t="s">
-        <v>187</v>
+        <v>143</v>
       </c>
       <c r="C39" t="s">
         <v>2</v>
@@ -2832,7 +2682,7 @@
         <v>4</v>
       </c>
       <c r="F39" t="s">
-        <v>188</v>
+        <v>144</v>
       </c>
       <c r="G39" t="s">
         <v>6</v>
@@ -2847,33 +2697,33 @@
         <v>9</v>
       </c>
       <c r="K39" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="L39" t="s">
-        <v>189</v>
+        <v>11</v>
       </c>
       <c r="M39" t="s">
-        <v>189</v>
+        <v>11</v>
       </c>
       <c r="N39" t="s">
         <v>12</v>
       </c>
       <c r="O39" t="s">
-        <v>187</v>
+        <v>143</v>
       </c>
       <c r="P39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q39" t="s">
-        <v>190</v>
+        <v>145</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>191</v>
+        <v>20</v>
       </c>
       <c r="B40" t="s">
-        <v>192</v>
+        <v>69</v>
       </c>
       <c r="C40" t="s">
         <v>2</v>
@@ -2885,7 +2735,7 @@
         <v>4</v>
       </c>
       <c r="F40" t="s">
-        <v>193</v>
+        <v>146</v>
       </c>
       <c r="G40" t="s">
         <v>6</v>
@@ -2897,36 +2747,36 @@
         <v>8</v>
       </c>
       <c r="J40" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="K40" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="L40" t="s">
-        <v>189</v>
+        <v>11</v>
       </c>
       <c r="M40" t="s">
-        <v>189</v>
+        <v>11</v>
       </c>
       <c r="N40" t="s">
         <v>12</v>
       </c>
       <c r="O40" t="s">
-        <v>194</v>
+        <v>121</v>
       </c>
       <c r="P40" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q40" t="s">
-        <v>195</v>
+        <v>68</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>196</v>
+        <v>147</v>
       </c>
       <c r="B41" t="s">
-        <v>197</v>
+        <v>148</v>
       </c>
       <c r="C41" t="s">
         <v>2</v>
@@ -2938,7 +2788,7 @@
         <v>4</v>
       </c>
       <c r="F41" t="s">
-        <v>198</v>
+        <v>149</v>
       </c>
       <c r="G41" t="s">
         <v>6</v>
@@ -2950,36 +2800,36 @@
         <v>8</v>
       </c>
       <c r="J41" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="K41" t="s">
         <v>10</v>
       </c>
       <c r="L41" t="s">
-        <v>189</v>
+        <v>11</v>
       </c>
       <c r="M41" t="s">
-        <v>189</v>
+        <v>11</v>
       </c>
       <c r="N41" t="s">
         <v>12</v>
       </c>
       <c r="O41" t="s">
-        <v>197</v>
+        <v>148</v>
       </c>
       <c r="P41" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q41" t="s">
-        <v>199</v>
+        <v>150</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>200</v>
+        <v>151</v>
       </c>
       <c r="B42" t="s">
-        <v>201</v>
+        <v>152</v>
       </c>
       <c r="C42" t="s">
         <v>2</v>
@@ -2991,7 +2841,7 @@
         <v>4</v>
       </c>
       <c r="F42" t="s">
-        <v>202</v>
+        <v>153</v>
       </c>
       <c r="G42" t="s">
         <v>6</v>
@@ -3003,36 +2853,36 @@
         <v>8</v>
       </c>
       <c r="J42" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="K42" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="L42" t="s">
-        <v>189</v>
+        <v>11</v>
       </c>
       <c r="M42" t="s">
-        <v>189</v>
+        <v>11</v>
       </c>
       <c r="N42" t="s">
         <v>12</v>
       </c>
       <c r="O42" t="s">
-        <v>201</v>
+        <v>152</v>
       </c>
       <c r="P42" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q42" t="s">
-        <v>203</v>
+        <v>154</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>204</v>
+        <v>155</v>
       </c>
       <c r="B43" t="s">
-        <v>205</v>
+        <v>91</v>
       </c>
       <c r="C43" t="s">
         <v>2</v>
@@ -3044,7 +2894,7 @@
         <v>4</v>
       </c>
       <c r="F43" t="s">
-        <v>206</v>
+        <v>156</v>
       </c>
       <c r="G43" t="s">
         <v>6</v>
@@ -3056,36 +2906,36 @@
         <v>8</v>
       </c>
       <c r="J43" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="K43" t="s">
         <v>10</v>
       </c>
       <c r="L43" t="s">
-        <v>207</v>
+        <v>11</v>
       </c>
       <c r="M43" t="s">
-        <v>207</v>
+        <v>157</v>
       </c>
       <c r="N43" t="s">
         <v>12</v>
       </c>
       <c r="O43" t="s">
-        <v>205</v>
+        <v>91</v>
       </c>
       <c r="P43" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q43" t="s">
-        <v>208</v>
+        <v>141</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>209</v>
+        <v>158</v>
       </c>
       <c r="B44" t="s">
-        <v>210</v>
+        <v>53</v>
       </c>
       <c r="C44" t="s">
         <v>2</v>
@@ -3097,7 +2947,7 @@
         <v>4</v>
       </c>
       <c r="F44" t="s">
-        <v>211</v>
+        <v>159</v>
       </c>
       <c r="G44" t="s">
         <v>6</v>
@@ -3109,36 +2959,36 @@
         <v>8</v>
       </c>
       <c r="J44" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="K44" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="L44" t="s">
-        <v>207</v>
+        <v>160</v>
       </c>
       <c r="M44" t="s">
-        <v>207</v>
+        <v>160</v>
       </c>
       <c r="N44" t="s">
         <v>12</v>
       </c>
       <c r="O44" t="s">
-        <v>210</v>
+        <v>53</v>
       </c>
       <c r="P44" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q44" t="s">
-        <v>212</v>
+        <v>51</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>213</v>
+        <v>161</v>
       </c>
       <c r="B45" t="s">
-        <v>214</v>
+        <v>162</v>
       </c>
       <c r="C45" t="s">
         <v>2</v>
@@ -3150,7 +3000,7 @@
         <v>4</v>
       </c>
       <c r="F45" t="s">
-        <v>215</v>
+        <v>163</v>
       </c>
       <c r="G45" t="s">
         <v>6</v>
@@ -3162,36 +3012,36 @@
         <v>8</v>
       </c>
       <c r="J45" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="K45" t="s">
         <v>10</v>
       </c>
       <c r="L45" t="s">
-        <v>216</v>
+        <v>160</v>
       </c>
       <c r="M45" t="s">
-        <v>216</v>
+        <v>160</v>
       </c>
       <c r="N45" t="s">
         <v>12</v>
       </c>
       <c r="O45" t="s">
-        <v>214</v>
+        <v>162</v>
       </c>
       <c r="P45" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q45" t="s">
-        <v>217</v>
+        <v>164</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>218</v>
+        <v>165</v>
       </c>
       <c r="B46" t="s">
-        <v>219</v>
+        <v>166</v>
       </c>
       <c r="C46" t="s">
         <v>2</v>
@@ -3203,7 +3053,7 @@
         <v>4</v>
       </c>
       <c r="F46" t="s">
-        <v>220</v>
+        <v>167</v>
       </c>
       <c r="G46" t="s">
         <v>6</v>
@@ -3215,36 +3065,36 @@
         <v>8</v>
       </c>
       <c r="J46" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="K46" t="s">
         <v>10</v>
       </c>
       <c r="L46" t="s">
-        <v>216</v>
+        <v>168</v>
       </c>
       <c r="M46" t="s">
-        <v>216</v>
+        <v>168</v>
       </c>
       <c r="N46" t="s">
         <v>12</v>
       </c>
       <c r="O46" t="s">
-        <v>219</v>
+        <v>166</v>
       </c>
       <c r="P46" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q46" t="s">
-        <v>221</v>
+        <v>169</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>222</v>
+        <v>170</v>
       </c>
       <c r="B47" t="s">
-        <v>59</v>
+        <v>171</v>
       </c>
       <c r="C47" t="s">
         <v>2</v>
@@ -3256,7 +3106,7 @@
         <v>4</v>
       </c>
       <c r="F47" t="s">
-        <v>223</v>
+        <v>172</v>
       </c>
       <c r="G47" t="s">
         <v>6</v>
@@ -3268,36 +3118,36 @@
         <v>8</v>
       </c>
       <c r="J47" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="K47" t="s">
         <v>10</v>
       </c>
       <c r="L47" t="s">
-        <v>216</v>
+        <v>173</v>
       </c>
       <c r="M47" t="s">
-        <v>216</v>
+        <v>173</v>
       </c>
       <c r="N47" t="s">
         <v>12</v>
       </c>
       <c r="O47" t="s">
-        <v>59</v>
+        <v>174</v>
       </c>
       <c r="P47" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q47" t="s">
-        <v>224</v>
+        <v>175</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>225</v>
+        <v>176</v>
       </c>
       <c r="B48" t="s">
-        <v>226</v>
+        <v>177</v>
       </c>
       <c r="C48" t="s">
         <v>2</v>
@@ -3309,7 +3159,7 @@
         <v>4</v>
       </c>
       <c r="F48" t="s">
-        <v>227</v>
+        <v>178</v>
       </c>
       <c r="G48" t="s">
         <v>6</v>
@@ -3321,36 +3171,36 @@
         <v>8</v>
       </c>
       <c r="J48" t="s">
-        <v>96</v>
+        <v>17</v>
       </c>
       <c r="K48" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="L48" t="s">
-        <v>228</v>
+        <v>179</v>
       </c>
       <c r="M48" t="s">
-        <v>228</v>
+        <v>179</v>
       </c>
       <c r="N48" t="s">
         <v>12</v>
       </c>
       <c r="O48" t="s">
-        <v>226</v>
+        <v>177</v>
       </c>
       <c r="P48" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q48" t="s">
-        <v>229</v>
+        <v>180</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>230</v>
+        <v>181</v>
       </c>
       <c r="B49" t="s">
-        <v>231</v>
+        <v>182</v>
       </c>
       <c r="C49" t="s">
         <v>2</v>
@@ -3362,7 +3212,7 @@
         <v>4</v>
       </c>
       <c r="F49" t="s">
-        <v>232</v>
+        <v>183</v>
       </c>
       <c r="G49" t="s">
         <v>6</v>
@@ -3374,81 +3224,81 @@
         <v>8</v>
       </c>
       <c r="J49" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="K49" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="L49" t="s">
-        <v>228</v>
+        <v>184</v>
       </c>
       <c r="M49" t="s">
-        <v>228</v>
+        <v>184</v>
       </c>
       <c r="N49" t="s">
         <v>12</v>
       </c>
       <c r="O49" t="s">
-        <v>231</v>
+        <v>182</v>
       </c>
       <c r="P49" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q49" t="s">
-        <v>233</v>
+        <v>185</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="s">
-        <v>234</v>
-      </c>
-      <c r="B50" t="s">
-        <v>235</v>
-      </c>
-      <c r="C50" t="s">
-        <v>2</v>
-      </c>
-      <c r="D50" t="s">
-        <v>3</v>
-      </c>
-      <c r="E50" t="s">
-        <v>4</v>
-      </c>
-      <c r="F50" t="s">
-        <v>236</v>
-      </c>
-      <c r="G50" t="s">
-        <v>6</v>
-      </c>
-      <c r="H50" t="s">
-        <v>7</v>
-      </c>
-      <c r="I50" t="s">
-        <v>8</v>
-      </c>
-      <c r="J50" t="s">
-        <v>9</v>
-      </c>
-      <c r="K50" t="s">
-        <v>10</v>
-      </c>
-      <c r="L50" t="s">
-        <v>237</v>
-      </c>
-      <c r="M50" t="s">
-        <v>237</v>
-      </c>
-      <c r="N50" t="s">
-        <v>12</v>
-      </c>
-      <c r="O50" t="s">
-        <v>235</v>
-      </c>
-      <c r="P50" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q50" t="s">
-        <v>238</v>
+      <c r="A50" t="s" s="2">
+        <v>0</v>
+      </c>
+      <c r="B50" t="s" s="2">
+        <v>186</v>
+      </c>
+      <c r="C50" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="D50" t="s" s="2">
+        <v>3</v>
+      </c>
+      <c r="E50" t="s" s="2">
+        <v>4</v>
+      </c>
+      <c r="F50" t="s" s="2">
+        <v>187</v>
+      </c>
+      <c r="G50" t="s" s="2">
+        <v>6</v>
+      </c>
+      <c r="H50" t="s" s="2">
+        <v>7</v>
+      </c>
+      <c r="I50" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="J50" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="K50" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="L50" t="s" s="2">
+        <v>188</v>
+      </c>
+      <c r="M50" t="s" s="2">
+        <v>188</v>
+      </c>
+      <c r="N50" t="s" s="2">
+        <v>12</v>
+      </c>
+      <c r="O50" t="s" s="2">
+        <v>186</v>
+      </c>
+      <c r="P50" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="Q50" t="s" s="2">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>